<commit_message>
Return #NUM! error instead of Infinity in some cases
We should do it in all cases to match Excel, but we
are not there yet.
</commit_message>
<xml_diff>
--- a/spec/test_data/GoTestSpreadsheet.xlsx
+++ b/spec/test_data/GoTestSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tamc/Documents/excel_to_code/spec/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE84AD66-9240-B441-A435-96CEB5B365B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FBE925-FBDE-F745-892A-C90747880BCE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="40800" windowHeight="22780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,7 +480,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,7 +537,10 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="e">
+        <f>1E+99*1E+99*1E+99*1E+99</f>
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>

</xml_diff>

<commit_message>
Go: improve the way formula are created (WIP)
</commit_message>
<xml_diff>
--- a/spec/test_data/GoTestSpreadsheet.xlsx
+++ b/spec/test_data/GoTestSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tamc/Documents/excel_to_code/spec/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FBE925-FBDE-F745-892A-C90747880BCE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460D5845-C789-4649-8DA0-918487A44945}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="40800" windowHeight="22780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>The basic types</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>The error types</t>
+  </si>
+  <si>
+    <t>Basic arithmetic</t>
   </si>
 </sst>
 </file>
@@ -477,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,7 +491,7 @@
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="b">
         <f>TRUE</f>
         <v>1</v>
@@ -506,7 +509,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -515,7 +518,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>123</v>
       </c>
@@ -524,7 +527,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3.1415000000000002</v>
       </c>
@@ -533,7 +536,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -542,8 +545,22 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f>B9+C9</f>
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Go: experiment with types in output
</commit_message>
<xml_diff>
--- a/spec/test_data/GoTestSpreadsheet.xlsx
+++ b/spec/test_data/GoTestSpreadsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tamc/Documents/excel_to_code/spec/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460D5845-C789-4649-8DA0-918487A44945}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1C4F6E-7D18-E347-B922-54FDACD9B6A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="40800" windowHeight="22780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -552,8 +552,8 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <f>B9+C9</f>
-        <v>2</v>
+        <f>B9+C9+3</f>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>1</v>

</xml_diff>